<commit_message>
Scrum Sheets updated : Most recent version is v1.4 . No updates to any other files
</commit_message>
<xml_diff>
--- a/Gradeup- Scrum_v1.3.xlsx
+++ b/Gradeup- Scrum_v1.3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="User stories" sheetId="1" r:id="rId1"/>
@@ -1165,7 +1165,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1380,11 +1379,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="309019472"/>
-        <c:axId val="309019864"/>
+        <c:axId val="297195920"/>
+        <c:axId val="297197488"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="309019472"/>
+        <c:axId val="297195920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1406,14 +1405,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="309019864"/>
+        <c:crossAx val="297197488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1421,7 +1419,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="309019864"/>
+        <c:axId val="297197488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1444,7 +1442,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1466,14 +1463,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="309019472"/>
+        <c:crossAx val="297195920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1785,7 +1781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -2276,8 +2272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2946,7 +2942,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3831,35 +3827,35 @@
         <v>1</v>
       </c>
       <c r="C4" s="15">
-        <f>B4+1</f>
+        <f t="shared" ref="C4:J4" si="0">B4+1</f>
         <v>2</v>
       </c>
       <c r="D4" s="13">
-        <f>C4+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E4" s="12">
-        <f>D4+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F4" s="15">
-        <f>E4+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="G4" s="16">
-        <f>F4+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H4" s="12">
-        <f>G4+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="I4" s="15">
-        <f>H4+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="J4" s="16">
-        <f>I4+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>

</xml_diff>